<commit_message>
Adjusted Tim and updated Placement Matrix
Added copy static to dist once for dev script
</commit_message>
<xml_diff>
--- a/Garden App/Placement Matrix.xlsx
+++ b/Garden App/Placement Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\open source\cg2020-group-picture-another-dimension\Garden App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F884E86A-BB51-4472-9B91-CD7487FAE020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C3E676-0B4E-4F91-809A-156E6A0CCA60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="345" windowWidth="23250" windowHeight="11385" xr2:uid="{F8C92782-3532-4DC7-B124-FC0059F4BC3B}"/>
+    <workbookView xWindow="29850" yWindow="1755" windowWidth="23250" windowHeight="11385" xr2:uid="{F8C92782-3532-4DC7-B124-FC0059F4BC3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1698B-C871-4654-8B79-F643E8D89EA0}">
   <dimension ref="B1:AP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,7 +1767,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
+      <c r="V33" s="3"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>

</xml_diff>

<commit_message>
New heads, accessibility team + rover
</commit_message>
<xml_diff>
--- a/Garden App/Placement Matrix.xlsx
+++ b/Garden App/Placement Matrix.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\open source\cg2020-group-picture-another-dimension\Garden App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C3E676-0B4E-4F91-809A-156E6A0CCA60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6A5846-8A1E-45B8-801B-8F5388ACA7D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29850" yWindow="1755" windowWidth="23250" windowHeight="11385" xr2:uid="{F8C92782-3532-4DC7-B124-FC0059F4BC3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8C92782-3532-4DC7-B124-FC0059F4BC3B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Placement Matrix" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +98,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -126,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -136,6 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1698B-C871-4654-8B79-F643E8D89EA0}">
   <dimension ref="B1:AP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="AZ12" sqref="AZ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>-19</v>
       </c>
@@ -542,7 +549,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -583,7 +590,7 @@
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -624,7 +631,7 @@
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -665,7 +672,7 @@
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>-15</v>
       </c>
@@ -709,7 +716,7 @@
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -750,7 +757,7 @@
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -791,7 +798,7 @@
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -832,7 +839,7 @@
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -873,7 +880,7 @@
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>-10</v>
       </c>
@@ -917,7 +924,7 @@
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -958,7 +965,7 @@
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -999,7 +1006,7 @@
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1040,7 +1047,7 @@
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1081,7 +1088,7 @@
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>-5</v>
       </c>
@@ -1125,7 +1132,7 @@
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
     </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1166,7 +1173,7 @@
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1207,7 +1214,7 @@
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
     </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1229,6 +1236,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
@@ -1247,7 +1255,7 @@
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
     </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1288,7 +1296,7 @@
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>0</v>
       </c>
@@ -1332,7 +1340,7 @@
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1373,7 +1381,7 @@
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
     </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1414,7 +1422,7 @@
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1424,7 +1432,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="L25" s="9"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1455,7 +1463,7 @@
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1496,7 +1504,7 @@
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
     </row>
-    <row r="27" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>5</v>
       </c>
@@ -1540,7 +1548,7 @@
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
     </row>
-    <row r="28" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1581,7 +1589,7 @@
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
     </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1596,6 +1604,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="3"/>
+      <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -1621,7 +1630,7 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
     </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1662,7 +1671,7 @@
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
     </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1703,7 +1712,7 @@
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
     </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>10</v>
       </c>
@@ -1747,7 +1756,7 @@
       <c r="AN32" s="1"/>
       <c r="AO32" s="1"/>
     </row>
-    <row r="33" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1788,7 +1797,7 @@
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
     </row>
-    <row r="34" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1801,6 +1810,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -1828,7 +1838,7 @@
       <c r="AN34" s="1"/>
       <c r="AO34" s="1"/>
     </row>
-    <row r="35" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1869,7 +1879,7 @@
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
     </row>
-    <row r="36" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1910,7 +1920,7 @@
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
     </row>
-    <row r="37" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>15</v>
       </c>
@@ -1954,7 +1964,7 @@
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
     </row>
-    <row r="38" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1995,7 +2005,7 @@
       <c r="AN38" s="1"/>
       <c r="AO38" s="1"/>
     </row>
-    <row r="39" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -2036,7 +2046,7 @@
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
     </row>
-    <row r="40" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2077,7 +2087,7 @@
       <c r="AN40" s="1"/>
       <c r="AO40" s="1"/>
     </row>
-    <row r="41" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2118,7 +2128,7 @@
       <c r="AN41" s="1"/>
       <c r="AO41" s="1"/>
     </row>
-    <row r="42" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>20</v>
       </c>
@@ -2162,7 +2172,7 @@
       <c r="AN42" s="1"/>
       <c r="AO42" s="1"/>
     </row>
-    <row r="43" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2203,7 +2213,7 @@
       <c r="AN43" s="1"/>
       <c r="AO43" s="1"/>
     </row>
-    <row r="44" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2244,7 +2254,7 @@
       <c r="AN44" s="1"/>
       <c r="AO44" s="1"/>
     </row>
-    <row r="45" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2285,7 +2295,7 @@
       <c r="AN45" s="1"/>
       <c r="AO45" s="1"/>
     </row>
-    <row r="46" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2326,7 +2336,7 @@
       <c r="AN46" s="1"/>
       <c r="AO46" s="1"/>
     </row>
-    <row r="47" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>25</v>
       </c>
@@ -2370,7 +2380,7 @@
       <c r="AN47" s="1"/>
       <c r="AO47" s="1"/>
     </row>
-    <row r="48" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2411,7 +2421,7 @@
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
     </row>
-    <row r="49" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2452,7 +2462,7 @@
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
     </row>
-    <row r="50" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2493,7 +2503,7 @@
       <c r="AN50" s="1"/>
       <c r="AO50" s="1"/>
     </row>
-    <row r="51" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2534,7 +2544,7 @@
       <c r="AN51" s="1"/>
       <c r="AO51" s="1"/>
     </row>
-    <row r="52" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>30</v>
       </c>
@@ -2578,7 +2588,7 @@
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
     </row>
-    <row r="53" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2619,7 +2629,7 @@
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
     </row>
-    <row r="54" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2660,10 +2670,10 @@
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
     </row>
-    <row r="55" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="E55" s="7"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2701,7 +2711,7 @@
       <c r="AN55" s="1"/>
       <c r="AO55" s="1"/>
     </row>
-    <row r="56" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2742,7 +2752,7 @@
       <c r="AN56" s="1"/>
       <c r="AO56" s="1"/>
     </row>
-    <row r="57" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2783,7 +2793,7 @@
       <c r="AN57" s="1"/>
       <c r="AO57" s="1"/>
     </row>
-    <row r="58" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>36</v>
       </c>

</xml_diff>